<commit_message>
Fixed xls/xlsx parsers. Changed main.py to vsat/selftest.py. Fixed excel files.
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12150" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12150" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="TESTCASES" sheetId="1" r:id="rId1"/>
-    <sheet name="HUB" sheetId="4" r:id="rId2"/>
-    <sheet name="VSAT" sheetId="5" r:id="rId3"/>
-    <sheet name="INFO" sheetId="2" r:id="rId4"/>
+    <sheet name="A-INFO" sheetId="2" r:id="rId1"/>
+    <sheet name="B-VSAT" sheetId="5" r:id="rId2"/>
+    <sheet name="C-HUB" sheetId="4" r:id="rId3"/>
+    <sheet name="D-TESTCASES" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -892,670 +892,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H65536"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="12" customWidth="1"/>
-    <col min="3" max="7" width="15.7109375" style="12" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="12" customWidth="1"/>
-    <col min="9" max="16" width="15.7109375" style="12" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" style="23" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="24" customFormat="1" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="26" t="s">
+    <row r="1" spans="1:3" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="B2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="26" t="s">
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="12">
-        <v>40000</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="12">
-        <v>512</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="12">
-        <v>4</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="J3" s="12">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>2</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="12">
-        <v>30000</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="12">
-        <v>2560</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" s="12">
-        <v>4</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>3</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="12">
-        <v>20000</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" s="12">
-        <v>1536</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" s="12">
-        <v>2</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="J5" s="12">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
-        <v>4</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="12">
-        <v>10000</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="12">
-        <v>1024</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="12">
-        <v>4</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J6" s="12">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
-        <v>5</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="12">
-        <v>8000</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="12">
-        <v>512</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="12">
-        <v>4</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="12">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>6</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="12">
-        <v>35000</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="12">
-        <v>1536</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="12">
-        <v>2</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="J8" s="12">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>7</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="12">
-        <v>20000</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="12">
-        <v>256</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="12">
-        <v>2</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>8</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="12">
-        <v>5000</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="12">
-        <v>512</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="12">
-        <v>4</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J10" s="12">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>9</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="12">
-        <v>10000</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="12">
-        <v>2560</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H11" s="12">
-        <v>2</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J11" s="12">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="12">
-        <v>15000</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="12">
-        <v>1024</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H12" s="12">
-        <v>2</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="J12" s="12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>11</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="12">
-        <v>30000</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="12">
-        <v>512</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="12">
-        <v>2</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="J13" s="12">
-        <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A65536"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" style="20" customWidth="1"/>
-    <col min="2" max="3" width="15.7109375" style="12"/>
-    <col min="4" max="7" width="15.7109375" style="20"/>
-    <col min="8" max="8" width="15.7109375" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="20">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="20">
-        <v>11</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="20">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="20">
-        <v>12</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="20">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="20">
-        <v>65</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="20">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="20">
-        <v>66</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="20">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="20">
-        <v>1006</v>
-      </c>
-    </row>
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -1763,98 +1194,667 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" sqref="A1:A65536"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="20" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" style="12"/>
+    <col min="4" max="7" width="15.7109375" style="20"/>
+    <col min="8" max="8" width="15.7109375" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="1" spans="1:8" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="20">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="20">
         <v>11</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="E4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="20">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="20">
         <v>12</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="F5" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="20">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="20">
+        <v>65</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="20">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="20">
+        <v>66</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="20">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="20">
+        <v>1006</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.7109375" style="12" customWidth="1"/>
+    <col min="3" max="7" width="15.7109375" style="12" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="12" customWidth="1"/>
+    <col min="9" max="16" width="15.7109375" style="12" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" style="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="24" customFormat="1" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="12">
+        <v>40000</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="12">
+        <v>512</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="12">
+        <v>4</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="12">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="12">
+        <v>30000</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="12">
+        <v>2560</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="12">
+        <v>4</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="12">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="12">
+        <v>20000</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1536</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="12">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="12">
+        <v>10000</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1024</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="12">
+        <v>4</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="12">
+        <v>8000</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="12">
+        <v>512</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="12">
+        <v>4</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>6</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="12">
+        <v>35000</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="12">
+        <v>1536</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="12">
+        <v>2</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>7</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="12">
+        <v>20000</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="12">
+        <v>256</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="12">
+        <v>2</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="12">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="12">
+        <v>5000</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="12">
+        <v>512</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="12">
+        <v>4</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" s="12">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="12">
+        <v>10000</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="12">
+        <v>2560</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="12">
+        <v>2</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="12">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="12">
+        <v>15000</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="12">
+        <v>1024</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="12">
+        <v>2</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12" s="12">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="12">
+        <v>30000</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="12">
+        <v>512</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="12">
+        <v>2</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" s="12">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Need to finish set ngnms workpoint, save data to excel file.
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="22995" windowHeight="10515" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22995" windowHeight="10515" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="A-INFO" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="96">
   <si>
     <t>OB symbol rate</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Number of received IB packets</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of OB retransmit packets </t>
-  </si>
-  <si>
     <t>Number of IB retransmit packets</t>
   </si>
   <si>
@@ -187,9 +184,6 @@
     <t>010.141.010.001</t>
   </si>
   <si>
-    <t>10.111.35.3</t>
-  </si>
-  <si>
     <t>10.111.35.4</t>
   </si>
   <si>
@@ -305,6 +299,12 @@
   </si>
   <si>
     <t>Tries timeout</t>
+  </si>
+  <si>
+    <t>192.168.140.76</t>
+  </si>
+  <si>
+    <t>Number of OB retransmit packets</t>
   </si>
 </sst>
 </file>
@@ -328,19 +328,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -609,7 +609,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -618,8 +618,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1060,54 +1060,54 @@
         <v>20</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" s="15">
         <v>1001</v>
@@ -1115,19 +1115,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" s="15">
         <v>11</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G4" s="15">
         <v>1002</v>
@@ -1135,19 +1135,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" s="15">
         <v>12</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G5" s="15">
         <v>1003</v>
@@ -1155,19 +1155,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" s="15">
         <v>65</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G6" s="15">
         <v>1004</v>
@@ -1175,16 +1175,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7" s="15">
         <v>66</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G7" s="15">
         <v>1005</v>
@@ -1192,16 +1192,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G8" s="15">
         <v>1006</v>
@@ -1216,9 +1216,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H8"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,244 +1239,240 @@
         <v>20</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>33</v>
-      </c>
       <c r="D1" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="27" t="s">
+      <c r="H1" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="C2" s="10">
         <v>3001</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="F2" s="10" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="G2" s="28">
-        <v>1001</v>
+        <v>1016</v>
       </c>
       <c r="H2" s="34">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I2" s="31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J2" s="12">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6">
         <v>3002</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G3" s="28">
         <v>1002</v>
       </c>
       <c r="H3" s="34">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I3" s="31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J3" s="12">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="6">
         <v>3003</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G4" s="28">
         <v>1003</v>
       </c>
       <c r="H4" s="34">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I4" s="31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J4" s="12">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="6">
         <v>3004</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G5" s="28">
         <v>1004</v>
       </c>
       <c r="H5" s="34">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I5" s="31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J5" s="12">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>75</v>
-      </c>
       <c r="B6" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="6">
         <v>3005</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G6" s="28">
         <v>1005</v>
       </c>
       <c r="H6" s="34">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I6" s="31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J6" s="12">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="6">
         <v>3009</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G7" s="28">
         <v>1009</v>
       </c>
       <c r="H7" s="34">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I7" s="31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J7" s="12">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>75</v>
-      </c>
       <c r="B8" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="6">
         <v>3010</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G8" s="28">
         <v>1010</v>
       </c>
       <c r="H8" s="34">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I8" s="31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J8" s="12">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1488,9 +1484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,7 +1527,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K1" s="23" t="s">
         <v>23</v>
@@ -1549,10 +1545,10 @@
         <v>27</v>
       </c>
       <c r="P1" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q1" s="23" t="s">
         <v>28</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1587,25 +1583,25 @@
         <v>22</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1613,31 +1609,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" s="7">
         <v>40000</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E3" s="7">
         <v>512</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H3" s="7">
         <v>4</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J3" s="7">
-        <v>600</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1648,25 +1644,25 @@
         <v>30000</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" s="7">
         <v>2560</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="H4" s="7">
         <v>4</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J4" s="7">
-        <v>400</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1677,25 +1673,25 @@
         <v>20000</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E5" s="7">
         <v>1536</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H5" s="7">
         <v>2</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J5" s="7">
-        <v>500</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1703,31 +1699,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" s="7">
         <v>10000</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" s="7">
         <v>1024</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H6" s="7">
         <v>4</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J6" s="7">
-        <v>200</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1738,25 +1734,25 @@
         <v>8000</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E7" s="7">
         <v>512</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H7" s="7">
         <v>4</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J7" s="7">
-        <v>500</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1764,31 +1760,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" s="7">
         <v>35000</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E8" s="7">
         <v>1536</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H8" s="7">
         <v>2</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J8" s="7">
-        <v>300</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1796,31 +1792,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" s="7">
         <v>20000</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E9" s="7">
         <v>256</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H9" s="7">
         <v>2</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J9" s="7">
-        <v>400</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1831,25 +1827,25 @@
         <v>5000</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E10" s="7">
         <v>512</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H10" s="7">
         <v>4</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J10" s="7">
-        <v>600</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1857,31 +1853,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" s="7">
         <v>10000</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E11" s="7">
         <v>2560</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H11" s="7">
         <v>2</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J11" s="7">
-        <v>600</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1892,25 +1888,25 @@
         <v>15000</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E12" s="7">
         <v>1024</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H12" s="7">
         <v>2</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J12" s="7">
-        <v>400</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1921,25 +1917,25 @@
         <v>30000</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E13" s="7">
         <v>512</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H13" s="7">
         <v>2</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J13" s="7">
-        <v>300</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>